<commit_message>
feat(ddl): 根据 excel 生成 ddl
</commit_message>
<xml_diff>
--- a/sql/sql.xlsx
+++ b/sql/sql.xlsx
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1280,7 +1280,9 @@
         <v>1</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="b">
         <v>1</v>

</xml_diff>